<commit_message>
minor fix on date
</commit_message>
<xml_diff>
--- a/data/project_timeline.xlsx
+++ b/data/project_timeline.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/linyang/Downloads/P8105/p8105_final_project/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Edward\Desktop\Data Science BISTP8105\p8105_final_project\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CE3E09D-D18A-2D4D-BE78-D739BFB4BA98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4431C2E4-4F7A-4B34-883E-A486C5B8E045}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5880" yWindow="5900" windowWidth="28040" windowHeight="17440" xr2:uid="{DFDE4875-0F51-C84A-AF2A-410677C3EE79}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="13320" xr2:uid="{DFDE4875-0F51-C84A-AF2A-410677C3EE79}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -97,9 +97,6 @@
     <t xml:space="preserve"> 12/11</t>
   </si>
   <si>
-    <t xml:space="preserve"> 11/16-11/19/</t>
-  </si>
-  <si>
     <t xml:space="preserve"> 11/20-11/21</t>
   </si>
   <si>
@@ -113,17 +110,21 @@
   </si>
   <si>
     <t xml:space="preserve"> 12/7-12/10</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 11/16-11/19</t>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -131,22 +132,29 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="10.5"/>
       <color rgb="FF333333"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF333333"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -178,7 +186,7 @@
     <xf numFmtId="16" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -194,7 +202,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -493,17 +501,17 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="15.6640625" customWidth="1"/>
     <col min="2" max="2" width="46.33203125" customWidth="1"/>
-    <col min="3" max="3" width="15.5" customWidth="1"/>
+    <col min="3" max="3" width="15.46484375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -514,7 +522,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>18</v>
       </c>
@@ -525,9 +533,9 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>4</v>
@@ -536,9 +544,9 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>5</v>
@@ -547,9 +555,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>6</v>
@@ -558,7 +566,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>19</v>
       </c>
@@ -569,9 +577,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>8</v>
@@ -580,9 +588,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>9</v>
@@ -591,9 +599,9 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>10</v>
@@ -602,7 +610,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>20</v>
       </c>
@@ -613,7 +621,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>20</v>
       </c>
@@ -625,6 +633,8 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>